<commit_message>
fieldsites corrected here and in google sheet
</commit_message>
<xml_diff>
--- a/MAP/European Network of Ethnobiology.xlsx
+++ b/MAP/European Network of Ethnobiology.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dauam-my.sharepoint.com/personal/jimena_mateo_uam_es/Documents/Documents/Estudios/Doctorado/Colaboraciones/European Network of Ethnobiology/european_ethnobiology/MAP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{D6427C8D-5A2E-4A27-BBF2-27E5667F7217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8725DB0E-CDDF-DB47-9C9C-29D9C7C74036}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{D6427C8D-5A2E-4A27-BBF2-27E5667F7217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D79B363-9180-8545-B318-59E8D658ECD7}"/>
   <bookViews>
-    <workbookView xWindow="5540" yWindow="960" windowWidth="29420" windowHeight="20640" xr2:uid="{590E6805-1AD1-4CD2-80C3-8D396DA581B3}"/>
+    <workbookView xWindow="-26140" yWindow="3220" windowWidth="24500" windowHeight="18380" xr2:uid="{590E6805-1AD1-4CD2-80C3-8D396DA581B3}"/>
   </bookViews>
   <sheets>
     <sheet name="European Network of Ethnobiolog" sheetId="1" r:id="rId1"/>
@@ -1768,15 +1768,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4968A0-2733-4B0E-9FFF-6A4702B1C1C4}">
   <dimension ref="A1:AH33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="26.1640625" customWidth="1"/>
-    <col min="4" max="4" width="33.83203125" customWidth="1"/>
-    <col min="8" max="8" width="36" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" customWidth="1"/>
+    <col min="8" max="8" width="4.6640625" style="1" customWidth="1"/>
+    <col min="11" max="13" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.2">

</xml_diff>